<commit_message>
- Add one-sided background subtraction controlled by the "object_type" in the constructor of "Track". Use "dark" to look for objects darker than the background, "light" for objects lighter than the background, "both" for both. The original intent was to help with spotlight reflections in the IR-lit dark trials, however it doesn't work because the reflection flickers, the flicker factors into the background and ends up creating both darker-than-background and lighter-than-background spots.
- Tweaked traceback reporting in "tracker.py" and "gui_main.py".
</commit_message>
<xml_diff>
--- a/settings/adult-schooling.xlsx
+++ b/settings/adult-schooling.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t xml:space="preserve">trial filter</t>
   </si>
@@ -49,6 +49,12 @@
     <t xml:space="preserve">bkg.contrast_factor</t>
   </si>
   <si>
+    <t xml:space="preserve">bkg.object_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“both”</t>
+  </si>
+  <si>
     <t xml:space="preserve">bkg.secondary_subtraction</t>
   </si>
   <si>
@@ -104,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">*dark*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'dark’</t>
   </si>
 </sst>
 </file>
@@ -246,16 +255,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="66.27"/>
   </cols>
@@ -325,31 +334,31 @@
       <c r="B6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
     <row r="8" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
+      <c r="B8" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,33 +366,32 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -392,10 +400,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -404,10 +412,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -416,10 +424,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>800</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -428,10 +436,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>150</v>
+        <v>800</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -440,10 +448,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -452,10 +460,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -464,10 +472,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2"/>
     </row>
@@ -476,10 +484,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -487,12 +495,13 @@
       <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="C20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
@@ -501,82 +510,110 @@
       <c r="B21" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="0" t="n">
-        <v>0.5</v>
+      <c r="C21" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>10</v>
-      </c>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Added "max_displacement" option to "Track" constructor. Value in pixels. If a fish moves by more than max_displacement between consecutive frames, its new position is set to NaN. Set to None or a negative value to disable.   However it's double-edged. A fish needs a NaN frame before it can jump to a far-away position, but if it does, it also needs a NaN frame before it can jump back to its true position.
</commit_message>
<xml_diff>
--- a/settings/adult-schooling.xlsx
+++ b/settings/adult-schooling.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t xml:space="preserve">trial filter</t>
   </si>
@@ -67,6 +67,9 @@
     <t xml:space="preserve">t_end</t>
   </si>
   <si>
+    <t xml:space="preserve">n_extra</t>
+  </si>
+  <si>
     <t xml:space="preserve">n_blur</t>
   </si>
   <si>
@@ -94,7 +97,10 @@
     <t xml:space="preserve">area_penalty</t>
   </si>
   <si>
-    <t xml:space="preserve">n_extra</t>
+    <t xml:space="preserve">max_displacement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
   </si>
   <si>
     <t xml:space="preserve">morph_transform</t>
@@ -255,13 +261,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
@@ -391,7 +397,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -403,7 +409,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -415,7 +421,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -427,7 +433,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -439,7 +445,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>800</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -451,7 +457,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>150</v>
+        <v>800</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -463,7 +469,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -475,7 +481,7 @@
         <v>22</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D18" s="2"/>
     </row>
@@ -487,7 +493,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -499,7 +505,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -507,12 +513,13 @@
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
@@ -521,98 +528,107 @@
       <c r="B22" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="0" t="n">
-        <v>0.5</v>
+      <c r="C22" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="D23" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="2" t="n">
-        <v>10</v>
-      </c>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C28" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
- Added bright spot removal in tracker and viewer. See the functions "Frame.get_spot_mask" and "Frame.remove_spots" and the tracker options "spot_threshold" (brightness difference with surroundings to be considered a bright spot) and "spot_dilate" (kernel size for bright spot dilation following adaptive thresholding).
- "max_displacement" now has to be a number -- set to negative value to disable.

- Added "max_merging_distance" option to "Track" constructor to control the maximum distance between two fish to be eligible for a merger in the next frame.
</commit_message>
<xml_diff>
--- a/settings/adult-schooling.xlsx
+++ b/settings/adult-schooling.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
   <si>
     <t xml:space="preserve">trial filter</t>
   </si>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">max_displacement</t>
   </si>
   <si>
-    <t xml:space="preserve">None</t>
+    <t xml:space="preserve">max_merging_distance</t>
   </si>
   <si>
     <t xml:space="preserve">morph_transform</t>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t xml:space="preserve">reversal_threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spot_threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spot_dilate</t>
   </si>
   <si>
     <t xml:space="preserve">*_SF_*</t>
@@ -261,15 +267,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="66.27"/>
@@ -516,8 +522,8 @@
       <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>26</v>
+      <c r="C21" s="2" t="n">
+        <v>-1</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -525,110 +531,184 @@
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>28</v>
-      </c>
+      <c r="B22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>0.5</v>
+        <v>27</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="D24" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="D25" s="2"/>
+      <c r="C25" s="0" t="n">
+        <v>-1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>12</v>
+        <v>32</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>3</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="C37" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>